<commit_message>
made code review to delete for loops. Rename some folders and files.Add folder for schema and db
</commit_message>
<xml_diff>
--- a/plans_test.xlsx
+++ b/plans_test.xlsx
@@ -453,7 +453,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2008-01-01</t>
+          <t>2009-01-01</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -468,7 +468,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-03-01</t>
+          <t>2026-03-01</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -483,7 +483,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2026-04-01</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -498,7 +498,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2027-04-01</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -513,7 +513,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-05-01</t>
+          <t>2028-05-01</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -528,7 +528,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-06-01</t>
+          <t>2029-06-01</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">

</xml_diff>